<commit_message>
add username to player aggregate report
</commit_message>
<xml_diff>
--- a/results/Player_Stats_2024-04-26.xlsx
+++ b/results/Player_Stats_2024-04-26.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,60 +436,65 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>riotIdGameName</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>game_minutes</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>kills</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>deaths</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>assists</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>kda</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>dmg</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>dpm</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>cs</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>csm</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>csd14</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>first_blood</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>solo_kills</t>
         </is>
@@ -501,40 +506,45 @@
           <t>FQCsPeyWrCVbkOy-aioApSwnW_idANVkq7u52thv3BmwQgWwypuAJZqwcjnZ7wb9SnAvf2rMxHTdDA</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Chaffles</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
         <v>51.28</v>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>4</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>8</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>2</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>0.75</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>29378</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>572.89</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>251</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>4.89</v>
       </c>
-      <c r="K2" t="n">
-        <v>0</v>
-      </c>
       <c r="L2" t="n">
         <v>0</v>
       </c>
       <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="n">
         <v>2</v>
       </c>
     </row>
@@ -544,40 +554,45 @@
           <t>23q-nAJ0xUpoHVVbSepaZY1GzaismXKT6alr90Bgevpn70aJaHStx7tmMR6mPkxB4bkdik9B3oeXKw</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>IamClone</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
         <v>51.28</v>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>5</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>15</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>9</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>0.93</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>20866</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>406.9</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>285</v>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>5.56</v>
       </c>
-      <c r="K3" t="n">
-        <v>0</v>
-      </c>
       <c r="L3" t="n">
         <v>0</v>
       </c>
       <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -587,40 +602,45 @@
           <t>J3jt2RM5ZbYKT5GB_cbqWS3IDxI-XsByyy85CCOYrrGThPpNLH3Kpee8tg6EP70BDWCX8vOGYA8GzA</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>백지 소라</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
         <v>51.28</v>
       </c>
-      <c r="C4" t="n">
+      <c r="D4" t="n">
         <v>2</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>12</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>6</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>0.67</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>21720</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>423.56</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>374</v>
       </c>
-      <c r="J4" t="n">
+      <c r="K4" t="n">
         <v>7.29</v>
       </c>
-      <c r="K4" t="n">
-        <v>0</v>
-      </c>
       <c r="L4" t="n">
         <v>0</v>
       </c>
       <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -630,40 +650,45 @@
           <t>Gz89RwpxHBEBAwxJ3Ky8PRJfhEz2oXrxeYQwxmHk-byAU8OxU-G7L7aZuoEoACp5IlZ40RGSF8llyw</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Ganjegreen</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
         <v>51.28</v>
       </c>
-      <c r="C5" t="n">
+      <c r="D5" t="n">
         <v>3</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>13</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>7</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>0.77</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>16316</v>
       </c>
-      <c r="H5" t="n">
+      <c r="I5" t="n">
         <v>318.17</v>
       </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
         <v>294</v>
       </c>
-      <c r="J5" t="n">
+      <c r="K5" t="n">
         <v>5.73</v>
       </c>
-      <c r="K5" t="n">
-        <v>0</v>
-      </c>
       <c r="L5" t="n">
         <v>0</v>
       </c>
       <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -673,40 +698,45 @@
           <t>SmaiuGaV6I0E4QgFuh2d0HxDi4vx_c8IYAxN20Xb5YToagxq4w6Md2SfnIRI-Msm1y5Zwahwy1UDGg</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Drewsph</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
         <v>51.28</v>
       </c>
-      <c r="C6" t="n">
+      <c r="D6" t="n">
         <v>3</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>14</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>5</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>0.57</v>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>6106</v>
       </c>
-      <c r="H6" t="n">
+      <c r="I6" t="n">
         <v>119.07</v>
       </c>
-      <c r="I6" t="n">
+      <c r="J6" t="n">
         <v>43</v>
       </c>
-      <c r="J6" t="n">
+      <c r="K6" t="n">
         <v>0.84</v>
       </c>
-      <c r="K6" t="n">
-        <v>0</v>
-      </c>
       <c r="L6" t="n">
         <v>0</v>
       </c>
       <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -716,40 +746,45 @@
           <t>Yx2hh29YAXaN7PN1NUcoNhhrKwxBCRNWnyFB2YrlwVS8lW-JtzUVefS_Ayp8kjJOu6XOg4IfikgyfQ</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>MAA DuckJugs</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
         <v>51.28</v>
       </c>
-      <c r="C7" t="n">
+      <c r="D7" t="n">
         <v>7</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>3</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>21</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>9.33</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>19066</v>
       </c>
-      <c r="H7" t="n">
+      <c r="I7" t="n">
         <v>371.8</v>
       </c>
-      <c r="I7" t="n">
+      <c r="J7" t="n">
         <v>300</v>
       </c>
-      <c r="J7" t="n">
+      <c r="K7" t="n">
         <v>5.85</v>
       </c>
-      <c r="K7" t="n">
-        <v>0</v>
-      </c>
       <c r="L7" t="n">
         <v>0</v>
       </c>
       <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -759,40 +794,45 @@
           <t>-4HhpLDD9bRO-iIGwL02erGrqHRj5Z4Qcd-ESGlEyQdEwQVpYagoBL4p-VYBE0MWUn1fPQjWLTguPg</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Empro</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
         <v>51.28</v>
       </c>
-      <c r="C8" t="n">
+      <c r="D8" t="n">
         <v>11</v>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
         <v>7</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>23</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>4.86</v>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>29285</v>
       </c>
-      <c r="H8" t="n">
+      <c r="I8" t="n">
         <v>571.08</v>
       </c>
-      <c r="I8" t="n">
+      <c r="J8" t="n">
         <v>338</v>
       </c>
-      <c r="J8" t="n">
+      <c r="K8" t="n">
         <v>6.59</v>
       </c>
-      <c r="K8" t="n">
-        <v>0</v>
-      </c>
       <c r="L8" t="n">
         <v>0</v>
       </c>
       <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
         <v>1</v>
       </c>
     </row>
@@ -802,40 +842,45 @@
           <t>OzEiE66LRYl-Sn_1EMdWFKlWaOrugGt0dJ3Om8Dizm_Ih9ovyRuLSqzruzseY5k9D1uFjnGk7hPBnA</t>
         </is>
       </c>
-      <c r="B9" t="n">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>redzawsome</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
         <v>51.28</v>
       </c>
-      <c r="C9" t="n">
+      <c r="D9" t="n">
         <v>19</v>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
         <v>2</v>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>10</v>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
         <v>14.5</v>
       </c>
-      <c r="G9" t="n">
+      <c r="H9" t="n">
         <v>32532</v>
       </c>
-      <c r="H9" t="n">
+      <c r="I9" t="n">
         <v>634.4</v>
       </c>
-      <c r="I9" t="n">
+      <c r="J9" t="n">
         <v>297</v>
       </c>
-      <c r="J9" t="n">
+      <c r="K9" t="n">
         <v>5.79</v>
       </c>
-      <c r="K9" t="n">
-        <v>0</v>
-      </c>
       <c r="L9" t="n">
         <v>0</v>
       </c>
       <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
         <v>3</v>
       </c>
     </row>
@@ -845,40 +890,45 @@
           <t>oXuV3otBsi99yHtIZLGd-m2Da7SuNESQJZB0FWkzVrSNqw6yJPwiD0EpTBe3L4Uw-pk8uLB1doTxGg</t>
         </is>
       </c>
-      <c r="B10" t="n">
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Oasis RSexy</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
         <v>51.28</v>
       </c>
-      <c r="C10" t="n">
+      <c r="D10" t="n">
         <v>16</v>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
         <v>4</v>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
         <v>25</v>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
         <v>10.25</v>
       </c>
-      <c r="G10" t="n">
+      <c r="H10" t="n">
         <v>35388</v>
       </c>
-      <c r="H10" t="n">
+      <c r="I10" t="n">
         <v>690.09</v>
       </c>
-      <c r="I10" t="n">
+      <c r="J10" t="n">
         <v>409</v>
       </c>
-      <c r="J10" t="n">
+      <c r="K10" t="n">
         <v>7.98</v>
       </c>
-      <c r="K10" t="n">
-        <v>0</v>
-      </c>
       <c r="L10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" t="n">
         <v>2</v>
       </c>
-      <c r="M10" t="n">
+      <c r="N10" t="n">
         <v>1</v>
       </c>
     </row>
@@ -888,40 +938,45 @@
           <t>KU-vzFFra5g7mn9TWm-FgZQQZkhGpo5PCG1WySTcAEOu-hUn4rPtgMHREJ0S7fsbuqpm6Pbiq5FaqQ</t>
         </is>
       </c>
-      <c r="B11" t="n">
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Doretha728</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
         <v>51.28</v>
       </c>
-      <c r="C11" t="n">
+      <c r="D11" t="n">
         <v>9</v>
       </c>
-      <c r="D11" t="n">
+      <c r="E11" t="n">
         <v>2</v>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
         <v>38</v>
       </c>
-      <c r="F11" t="n">
+      <c r="G11" t="n">
         <v>23.5</v>
       </c>
-      <c r="G11" t="n">
+      <c r="H11" t="n">
         <v>26323</v>
       </c>
-      <c r="H11" t="n">
+      <c r="I11" t="n">
         <v>513.3200000000001</v>
       </c>
-      <c r="I11" t="n">
+      <c r="J11" t="n">
         <v>59</v>
       </c>
-      <c r="J11" t="n">
+      <c r="K11" t="n">
         <v>1.15</v>
       </c>
-      <c r="K11" t="n">
-        <v>0</v>
-      </c>
       <c r="L11" t="n">
         <v>0</v>
       </c>
       <c r="M11" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" t="n">
         <v>1</v>
       </c>
     </row>
@@ -931,40 +986,45 @@
           <t>-6WdjgiRoO8t7wtr-wt4stuOSt6DZJ1whJfdzlNJonZGx8nj77mSwJr7MtnHpo_VP3XSJ0URl9hIEQ</t>
         </is>
       </c>
-      <c r="B12" t="n">
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>HPZ Tea Jay</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
         <v>68.18000000000001</v>
       </c>
-      <c r="C12" t="n">
+      <c r="D12" t="n">
         <v>6</v>
       </c>
-      <c r="D12" t="n">
+      <c r="E12" t="n">
         <v>8</v>
       </c>
-      <c r="E12" t="n">
+      <c r="F12" t="n">
         <v>12</v>
       </c>
-      <c r="F12" t="n">
+      <c r="G12" t="n">
         <v>2.25</v>
       </c>
-      <c r="G12" t="n">
+      <c r="H12" t="n">
         <v>33095</v>
       </c>
-      <c r="H12" t="n">
+      <c r="I12" t="n">
         <v>485.41</v>
       </c>
-      <c r="I12" t="n">
+      <c r="J12" t="n">
         <v>395</v>
       </c>
-      <c r="J12" t="n">
+      <c r="K12" t="n">
         <v>5.79</v>
       </c>
-      <c r="K12" t="n">
-        <v>0</v>
-      </c>
       <c r="L12" t="n">
         <v>0</v>
       </c>
       <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="n">
         <v>3</v>
       </c>
     </row>
@@ -974,42 +1034,47 @@
           <t>ZaFqIgTOw6WcgV-BbbTIHyq9ypzqO58N-By8VyGZwQbV5H7m3_Z-VkBA6hhdMkPNqUgxcDS3Dy1LVQ</t>
         </is>
       </c>
-      <c r="B13" t="n">
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>JustaWittleGuy</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
         <v>68.18000000000001</v>
       </c>
-      <c r="C13" t="n">
+      <c r="D13" t="n">
         <v>8</v>
       </c>
-      <c r="D13" t="n">
+      <c r="E13" t="n">
         <v>6</v>
       </c>
-      <c r="E13" t="n">
+      <c r="F13" t="n">
         <v>25</v>
       </c>
-      <c r="F13" t="n">
+      <c r="G13" t="n">
         <v>5.5</v>
       </c>
-      <c r="G13" t="n">
+      <c r="H13" t="n">
         <v>32204</v>
       </c>
-      <c r="H13" t="n">
+      <c r="I13" t="n">
         <v>472.34</v>
       </c>
-      <c r="I13" t="n">
+      <c r="J13" t="n">
         <v>411</v>
       </c>
-      <c r="J13" t="n">
+      <c r="K13" t="n">
         <v>6.03</v>
       </c>
-      <c r="K13" t="n">
-        <v>0</v>
-      </c>
       <c r="L13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13" t="n">
         <v>1</v>
       </c>
+      <c r="N13" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -1017,40 +1082,45 @@
           <t>-WIu7G0rI7-LnoZ58zxl5S_TehtKdgisk4UBSh8G_-szNkce75UUGxnrQcyh4CyPPErTuHE32vIxzg</t>
         </is>
       </c>
-      <c r="B14" t="n">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>CrimsonYoni</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
         <v>68.18000000000001</v>
       </c>
-      <c r="C14" t="n">
+      <c r="D14" t="n">
         <v>6</v>
       </c>
-      <c r="D14" t="n">
+      <c r="E14" t="n">
         <v>7</v>
       </c>
-      <c r="E14" t="n">
+      <c r="F14" t="n">
         <v>20</v>
       </c>
-      <c r="F14" t="n">
+      <c r="G14" t="n">
         <v>3.71</v>
       </c>
-      <c r="G14" t="n">
+      <c r="H14" t="n">
         <v>29731</v>
       </c>
-      <c r="H14" t="n">
+      <c r="I14" t="n">
         <v>436.07</v>
       </c>
-      <c r="I14" t="n">
+      <c r="J14" t="n">
         <v>363</v>
       </c>
-      <c r="J14" t="n">
+      <c r="K14" t="n">
         <v>5.32</v>
       </c>
-      <c r="K14" t="n">
-        <v>0</v>
-      </c>
       <c r="L14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" t="n">
         <v>1</v>
       </c>
-      <c r="M14" t="n">
+      <c r="N14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1060,40 +1130,45 @@
           <t>W5XJAD7byGBFpxtgh5Zn7-VcZ3pnKaAInHHyq3S0fLGIlU2c6Fq_dGfx_r-cBw99muBdikoTWsiVhQ</t>
         </is>
       </c>
-      <c r="B15" t="n">
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>agateo</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
         <v>68.18000000000001</v>
       </c>
-      <c r="C15" t="n">
+      <c r="D15" t="n">
         <v>22</v>
       </c>
-      <c r="D15" t="n">
+      <c r="E15" t="n">
         <v>6</v>
       </c>
-      <c r="E15" t="n">
+      <c r="F15" t="n">
         <v>12</v>
       </c>
-      <c r="F15" t="n">
+      <c r="G15" t="n">
         <v>5.67</v>
       </c>
-      <c r="G15" t="n">
+      <c r="H15" t="n">
         <v>61074</v>
       </c>
-      <c r="H15" t="n">
+      <c r="I15" t="n">
         <v>895.78</v>
       </c>
-      <c r="I15" t="n">
+      <c r="J15" t="n">
         <v>480</v>
       </c>
-      <c r="J15" t="n">
+      <c r="K15" t="n">
         <v>7.04</v>
       </c>
-      <c r="K15" t="n">
-        <v>0</v>
-      </c>
       <c r="L15" t="n">
         <v>0</v>
       </c>
       <c r="M15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1103,40 +1178,45 @@
           <t>uAzuWCCd6j0k0vqec-9c4W9cZCh_f73MwBb8kQOGW-WZJPJJnRwbF8cyj2cH_y49rfu6ja2oBjmtBw</t>
         </is>
       </c>
-      <c r="B16" t="n">
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Abraxo</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
         <v>68.18000000000001</v>
       </c>
-      <c r="C16" t="n">
+      <c r="D16" t="n">
         <v>3</v>
       </c>
-      <c r="D16" t="n">
+      <c r="E16" t="n">
         <v>4</v>
       </c>
-      <c r="E16" t="n">
+      <c r="F16" t="n">
         <v>30</v>
       </c>
-      <c r="F16" t="n">
+      <c r="G16" t="n">
         <v>8.25</v>
       </c>
-      <c r="G16" t="n">
+      <c r="H16" t="n">
         <v>13407</v>
       </c>
-      <c r="H16" t="n">
+      <c r="I16" t="n">
         <v>196.64</v>
       </c>
-      <c r="I16" t="n">
+      <c r="J16" t="n">
         <v>60</v>
       </c>
-      <c r="J16" t="n">
+      <c r="K16" t="n">
         <v>0.88</v>
       </c>
-      <c r="K16" t="n">
-        <v>0</v>
-      </c>
       <c r="L16" t="n">
         <v>0</v>
       </c>
       <c r="M16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1146,40 +1226,45 @@
           <t>zGbCwhM4U37_lqlbGOEQI5nPPR3fUs-4JosQuvksL0Wzc-HOZNsBX_spcDzmRPdUO6y0ynFCIyS9eg</t>
         </is>
       </c>
-      <c r="B17" t="n">
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Oasis psychotikk</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
         <v>68.18000000000001</v>
       </c>
-      <c r="C17" t="n">
+      <c r="D17" t="n">
         <v>6</v>
       </c>
-      <c r="D17" t="n">
+      <c r="E17" t="n">
         <v>7</v>
       </c>
-      <c r="E17" t="n">
+      <c r="F17" t="n">
         <v>5</v>
       </c>
-      <c r="F17" t="n">
+      <c r="G17" t="n">
         <v>1.57</v>
       </c>
-      <c r="G17" t="n">
+      <c r="H17" t="n">
         <v>42542</v>
       </c>
-      <c r="H17" t="n">
+      <c r="I17" t="n">
         <v>623.97</v>
       </c>
-      <c r="I17" t="n">
+      <c r="J17" t="n">
         <v>553</v>
       </c>
-      <c r="J17" t="n">
+      <c r="K17" t="n">
         <v>8.109999999999999</v>
       </c>
-      <c r="K17" t="n">
-        <v>0</v>
-      </c>
       <c r="L17" t="n">
         <v>0</v>
       </c>
       <c r="M17" t="n">
+        <v>0</v>
+      </c>
+      <c r="N17" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1189,40 +1274,45 @@
           <t>r2IGDxPoDHE3UvFgheESemF-I9vAzWmaOFV91-Hb0r1AaIr8qZCWGvpatJnYwb-ZdMQ8onUTvh7F0A</t>
         </is>
       </c>
-      <c r="B18" t="n">
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Bug</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
         <v>68.18000000000001</v>
       </c>
-      <c r="C18" t="n">
+      <c r="D18" t="n">
         <v>8</v>
       </c>
-      <c r="D18" t="n">
+      <c r="E18" t="n">
         <v>11</v>
       </c>
-      <c r="E18" t="n">
+      <c r="F18" t="n">
         <v>8</v>
       </c>
-      <c r="F18" t="n">
+      <c r="G18" t="n">
         <v>1.45</v>
       </c>
-      <c r="G18" t="n">
+      <c r="H18" t="n">
         <v>16095</v>
       </c>
-      <c r="H18" t="n">
+      <c r="I18" t="n">
         <v>236.07</v>
       </c>
-      <c r="I18" t="n">
+      <c r="J18" t="n">
         <v>317</v>
       </c>
-      <c r="J18" t="n">
+      <c r="K18" t="n">
         <v>4.65</v>
       </c>
-      <c r="K18" t="n">
-        <v>0</v>
-      </c>
       <c r="L18" t="n">
         <v>0</v>
       </c>
       <c r="M18" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1232,40 +1322,45 @@
           <t>CJFmfl--EjAIuNJ43ttUZR2DQjYYj9rY4feweHwAPJEFYblrjlYFYipPC8RkrUpHEmtUlkNQdq7wqA</t>
         </is>
       </c>
-      <c r="B19" t="n">
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>SimonLowell</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
         <v>68.18000000000001</v>
       </c>
-      <c r="C19" t="n">
+      <c r="D19" t="n">
         <v>6</v>
       </c>
-      <c r="D19" t="n">
+      <c r="E19" t="n">
         <v>7</v>
       </c>
-      <c r="E19" t="n">
+      <c r="F19" t="n">
         <v>13</v>
       </c>
-      <c r="F19" t="n">
+      <c r="G19" t="n">
         <v>2.71</v>
       </c>
-      <c r="G19" t="n">
+      <c r="H19" t="n">
         <v>61179</v>
       </c>
-      <c r="H19" t="n">
+      <c r="I19" t="n">
         <v>897.3200000000001</v>
       </c>
-      <c r="I19" t="n">
+      <c r="J19" t="n">
         <v>447</v>
       </c>
-      <c r="J19" t="n">
+      <c r="K19" t="n">
         <v>6.56</v>
       </c>
-      <c r="K19" t="n">
-        <v>0</v>
-      </c>
       <c r="L19" t="n">
         <v>0</v>
       </c>
       <c r="M19" t="n">
+        <v>0</v>
+      </c>
+      <c r="N19" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1275,40 +1370,45 @@
           <t>FUyGrN_QbW6A-Tg-zPBsUuBYyWS6jmIsrvM5p5swd31CqeoLjwJEhndAhueRZsU5Stfs3_U7fyyqGg</t>
         </is>
       </c>
-      <c r="B20" t="n">
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>bezzaboyo</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
         <v>68.18000000000001</v>
       </c>
-      <c r="C20" t="n">
+      <c r="D20" t="n">
         <v>11</v>
       </c>
-      <c r="D20" t="n">
+      <c r="E20" t="n">
         <v>9</v>
       </c>
-      <c r="E20" t="n">
+      <c r="F20" t="n">
         <v>10</v>
       </c>
-      <c r="F20" t="n">
+      <c r="G20" t="n">
         <v>2.33</v>
       </c>
-      <c r="G20" t="n">
+      <c r="H20" t="n">
         <v>43867</v>
       </c>
-      <c r="H20" t="n">
+      <c r="I20" t="n">
         <v>643.4</v>
       </c>
-      <c r="I20" t="n">
+      <c r="J20" t="n">
         <v>551</v>
       </c>
-      <c r="J20" t="n">
+      <c r="K20" t="n">
         <v>8.08</v>
       </c>
-      <c r="K20" t="n">
-        <v>0</v>
-      </c>
       <c r="L20" t="n">
         <v>0</v>
       </c>
       <c r="M20" t="n">
+        <v>0</v>
+      </c>
+      <c r="N20" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1318,40 +1418,45 @@
           <t>b9Dv3dTtRVGgBQvpJgu5tkclCN8VyFqO6KPRzKG8Wbo_yR_JAm2CnhcTqw4_8q3mktm8tgGHkyxVTA</t>
         </is>
       </c>
-      <c r="B21" t="n">
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Oasis Jags</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
         <v>68.18000000000001</v>
       </c>
-      <c r="C21" t="n">
-        <v>0</v>
-      </c>
       <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="n">
         <v>11</v>
       </c>
-      <c r="E21" t="n">
+      <c r="F21" t="n">
         <v>20</v>
       </c>
-      <c r="F21" t="n">
+      <c r="G21" t="n">
         <v>1.82</v>
       </c>
-      <c r="G21" t="n">
+      <c r="H21" t="n">
         <v>10416</v>
       </c>
-      <c r="H21" t="n">
+      <c r="I21" t="n">
         <v>152.77</v>
       </c>
-      <c r="I21" t="n">
+      <c r="J21" t="n">
         <v>88</v>
       </c>
-      <c r="J21" t="n">
+      <c r="K21" t="n">
         <v>1.29</v>
       </c>
-      <c r="K21" t="n">
-        <v>0</v>
-      </c>
       <c r="L21" t="n">
         <v>0</v>
       </c>
       <c r="M21" t="n">
+        <v>0</v>
+      </c>
+      <c r="N21" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>